<commit_message>
CDS curation phs tc 1-10
</commit_message>
<xml_diff>
--- a/InputFiles/CCDI/TC08_CCDI_PHS-Accession-phs002620_Institution-NCI_LibSelec-PolyA.xlsx
+++ b/InputFiles/CCDI/TC08_CCDI_PHS-Accession-phs002620_Institution-NCI_LibSelec-PolyA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Desktop\MarchBranch\Commons_Automation\InputFiles\CCDI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A08A4B15-C7A5-4E96-A58A-3C024350E433}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CC9B1D3-DE68-4958-9792-4BE1F03E493F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
@@ -62,624 +62,6 @@
   </si>
   <si>
     <t>FilesTab</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-Match (st:study)
-where st.phs_accession in ['phs002518']   
-Call {
-with st
-MATCH (file:clinical_measure_file)
-MATCH (p:participant)-[:of_clinical_measure_file]-(file)
-MATCH (st)&lt;-[:of_participant]-(p)
-OPTIONAL MATCH (p)&lt;-[:of_sample]-(sm:sample)
-OPTIONAL MATCH (st)&lt;-[:of_publication]-(pub:publication)
-OPTIONAL MATCH (p)&lt;-[:of_diagnosis]-(dg:diagnosis)
-OPTIONAL MATCH (p)&lt;-[:of_follow_up]-(fu:follow_up)
-OPTIONAL MATCH (st)&lt;-[:of_study_personnel]-(stp:study_personnel)
-OPTIONAL MATCH (st)&lt;-[:of_study_funding]-(stf:study_funding)
-UNWIND apoc.text.split(p.ethnicity, ';') AS ethnicities
-UNWIND apoc.text.split(p.race, ';') AS races
-RETURN DISTINCT
-  file.id as id,
-  p.id as pid,
-  file.clinical_measure_file_id AS file_id,
-  file.dcf_indexd_guid AS guid,
-  file.file_name AS file_name,
-  'Clinical data' AS file_category,
-  file.file_type AS file_type,
-  file.file_description AS file_description,
-  file.file_size AS file_size,
-  file.md5sum AS md5sum,
-  st.study_id AS study_id,
-  st.phs_accession as phs_accession,
-  st.study_acronym as study_acronym,
-  st.study_short_title as study_short_title,
-  p.participant_id AS participant_id,
-  null AS sample_id,
-  null as combined_filters,
-  COLLECT(DISTINCT {
-      race: races,
-      sex_at_birth: p.sex_at_birth,
-      ethnicity: ethnicities
-  }) AS participant_filters,
-  COLLECT(DISTINCT {
-      age_at_diagnosis: dg.age_at_diagnosis,
-      diagnosis_anatomic_site: dg.anatomic_site,
-      disease_phase: dg.disease_phase,
-      diagnosis_classification_system: dg.diagnosis_classification_system,
-      diagnosis_verification_status: dg.diagnosis_verification_status,
-      diagnosis_basis: dg.diagnosis_basis,
-      diagnosis_comment: dg.diagnosis_comment,
-      diagnosis_classification: dg.diagnosis_classification
-  }) AS diagnosis_filters,
-  COLLECT(DISTINCT fu.vital_status) as vital_status,
-  COLLECT(DISTINCT {
-      sample_anatomic_site: sm.anatomic_site,
-      participant_age_at_collection: sm.participant_age_at_collection,
-      sample_tumor_status: sm.sample_tumor_status,
-      tumor_classification: sm.tumor_classification
-  }) AS sample_filters,
-  COLLECT(DISTINCT stf.grant_id) as grant_id,
-  COLLECT(DISTINCT stp.institution) as institution,      
-  null AS library_selection,
-  null AS library_source,
-  null AS library_strategy
-UNION ALL
-with st
-MATCH (file:methylation_array_file)
-MATCH (p:participant)&lt;-[:of_sample]-(sm1:sample)&lt;-[*0..2]-(sm:sample)&lt;-[:of_methylation_array_file]-(file)
-MATCH (st)&lt;-[:of_participant]-(p)
-OPTIONAL MATCH (st)&lt;-[:of_publication]-(pub:publication)
-OPTIONAL MATCH (p)&lt;-[:of_diagnosis]-(dg:diagnosis)
-OPTIONAL MATCH (p)&lt;-[:of_follow_up]-(fu:follow_up)
-OPTIONAL MATCH (st)&lt;-[:of_study_personnel]-(stp:study_personnel)
-OPTIONAL MATCH (st)&lt;-[:of_study_funding]-(stf:study_funding)
-UNWIND apoc.text.split(p.ethnicity, ';') AS ethnicities
-UNWIND apoc.text.split(p.race, ';') AS races
-with file, p, sm1, sm, st, ethnicities, races, fu, dg, stf, stp
-RETURN DISTINCT
-  file.id as id,
-  p.id as pid,
-  file.methylation_array_file_id AS file_id,
-  file.dcf_indexd_guid AS guid,
-  file.file_name AS file_name,
-  'Methylation array' AS file_category,
-  file.file_type AS file_type,
-  file.file_description AS file_description,
-  file.file_size AS file_size,
-  file.md5sum AS md5sum,
-  st.study_id AS study_id,
-  st.phs_accession as phs_accession,
-  st.study_acronym as study_acronym,
-  st.study_short_title as study_short_title,
-  p.participant_id AS participant_id,
-  CASE sm1.sample_id WHEN sm.sample_id THEN sm.sample_id
-            ELSE sm1.sample_id + ',' + sm.sample_id END AS sample_id,
-  null as combined_filters,
-  COLLECT(DISTINCT {
-      race: races,
-      sex_at_birth: p.sex_at_birth,
-      ethnicity: ethnicities
-  }) AS participant_filters,
-  COLLECT(DISTINCT {
-      age_at_diagnosis: dg.age_at_diagnosis,
-      diagnosis_anatomic_site: dg.anatomic_site,
-      disease_phase: dg.disease_phase,
-      diagnosis_classification_system: dg.diagnosis_classification_system,
-      diagnosis_verification_status: dg.diagnosis_verification_status,
-      diagnosis_basis: dg.diagnosis_basis,
-      diagnosis_comment: dg.diagnosis_comment,
-      diagnosis_classification: dg.diagnosis_classification
-  }) AS diagnosis_filters,
-  COLLECT(DISTINCT fu.vital_status) as vital_status,
-  CASE sm1.sample_id WHEN sm.sample_id THEN COLLECT(DISTINCT {
-                              sample_anatomic_site: sm.anatomic_site,
-                              participant_age_at_collection: sm.participant_age_at_collection,
-                              sample_tumor_status: sm.sample_tumor_status,
-                              tumor_classification: sm.tumor_classification
-                          })
-            ELSE apoc.coll.union(COLLECT(DISTINCT {
-                              sample_anatomic_site: sm1.anatomic_site,
-                              participant_age_at_collection: sm1.participant_age_at_collection,
-                              sample_tumor_status: sm1.sample_tumor_status,
-                              tumor_classification: sm1.tumor_classification
-                          }), COLLECT(DISTINCT {
-                              sample_anatomic_site: sm.anatomic_site,
-                              participant_age_at_collection: sm.participant_age_at_collection,
-                              sample_tumor_status: sm.sample_tumor_status,
-                              tumor_classification: sm.tumor_classification
-                          })) END AS sample_filters,
-  COLLECT(DISTINCT stf.grant_id) as grant_id,
-  COLLECT(DISTINCT stp.institution) as institution,
-  null AS library_selection,
-  null AS library_source,
-  null AS library_strategy
-UNION ALL
-with st
-MATCH (file:pathology_file)
-MATCH (p:participant)&lt;-[:of_sample]-(sm1:sample)&lt;-[*0..2]-(sm:sample)&lt;-[:of_pathology_file]-(file)
-MATCH (st)&lt;-[:of_participant]-(p)
-OPTIONAL MATCH (st)&lt;-[:of_publication]-(pub:publication)
-OPTIONAL MATCH (p)&lt;-[:of_diagnosis]-(dg:diagnosis)
-OPTIONAL MATCH (p)&lt;-[:of_follow_up]-(fu:follow_up)
-OPTIONAL MATCH (st)&lt;-[:of_study_personnel]-(stp:study_personnel)
-OPTIONAL MATCH (st)&lt;-[:of_study_funding]-(stf:study_funding)
-UNWIND apoc.text.split(p.ethnicity, ';') AS ethnicities
-UNWIND apoc.text.split(p.race, ';') AS races
-with file, p, sm1, sm, st, ethnicities, races, fu, dg, stf, stp
-RETURN DISTINCT
-  file.id as id,
-  p.id as pid,
-  file.pathology_file_id AS file_id,
-  file.dcf_indexd_guid AS guid,
-  file.file_name AS file_name,
-  'Pathology imaging' AS file_category,
-  file.file_type AS file_type,
-  file.file_description AS file_description,
-  file.file_size AS file_size,
-  file.md5sum AS md5sum,
-  st.study_id AS study_id,
-  st.phs_accession as phs_accession,
-  st.study_acronym as study_acronym,
-  st.study_short_title as study_short_title,
-  p.participant_id AS participant_id,
-  CASE sm1.sample_id WHEN sm.sample_id THEN sm.sample_id
-            ELSE sm1.sample_id + ',' + sm.sample_id END AS sample_id,
-  null as combined_filters,
-  COLLECT(DISTINCT {
-      race: races,
-      sex_at_birth: p.sex_at_birth,
-      ethnicity: ethnicities
-  }) AS participant_filters,
-  COLLECT(DISTINCT {
-      age_at_diagnosis: dg.age_at_diagnosis,
-      diagnosis_anatomic_site: dg.anatomic_site,
-      disease_phase: dg.disease_phase,
-      diagnosis_classification_system: dg.diagnosis_classification_system,
-      diagnosis_verification_status: dg.diagnosis_verification_status,
-      diagnosis_basis: dg.diagnosis_basis,
-      diagnosis_comment: dg.diagnosis_comment,
-      diagnosis_classification: dg.diagnosis_classification
-  }) AS diagnosis_filters,
-  COLLECT(DISTINCT fu.vital_status) as vital_status,
-  CASE sm1.sample_id WHEN sm.sample_id THEN COLLECT(DISTINCT {
-                              sample_anatomic_site: sm.anatomic_site,
-                              participant_age_at_collection: sm.participant_age_at_collection,
-                              sample_tumor_status: sm.sample_tumor_status,
-                              tumor_classification: sm.tumor_classification
-                          })
-            ELSE apoc.coll.union(COLLECT(DISTINCT {
-                              sample_anatomic_site: sm1.anatomic_site,
-                              participant_age_at_collection: sm1.participant_age_at_collection,
-                              sample_tumor_status: sm1.sample_tumor_status,
-                              tumor_classification: sm1.tumor_classification
-                          }), COLLECT(DISTINCT {
-                              sample_anatomic_site: sm.anatomic_site,
-                              participant_age_at_collection: sm.participant_age_at_collection,
-                              sample_tumor_status: sm.sample_tumor_status,
-                              tumor_classification: sm.tumor_classification
-                          })) END AS sample_filters,
-  COLLECT(DISTINCT stf.grant_id) as grant_id,
-  COLLECT(DISTINCT stp.institution) as institution,
-  file.library_selection AS library_selection,
-  file.library_source AS library_source,
-  file.library_strategy AS library_strategy
-UNION ALL
-with st
-MATCH (file:radiology_file)
-MATCH (p:participant)&lt;-[:of_radiology_file]-(file)
-MATCH (st)&lt;-[:of_participant]-(p)
-OPTIONAL MATCH (p)&lt;-[:of_sample]-(sm:sample)
-OPTIONAL MATCH (st)&lt;-[:of_publication]-(pub:publication)
-OPTIONAL MATCH (p)&lt;-[:of_diagnosis]-(dg:diagnosis)
-OPTIONAL MATCH (p)&lt;-[:of_follow_up]-(fu:follow_up)
-OPTIONAL MATCH (st)&lt;-[:of_study_personnel]-(stp:study_personnel)
-OPTIONAL MATCH (st)&lt;-[:of_study_funding]-(stf:study_funding)
-UNWIND apoc.text.split(p.ethnicity, ';') AS ethnicities
-UNWIND apoc.text.split(p.race, ';') AS races
-RETURN DISTINCT
-  file.id as id,
-  p.id as pid,
-  file.radiology_file_id AS file_id,
-  file.dcf_indexd_guid AS guid,
-  file.file_name AS file_name,
-  'Radiology imaging' AS file_category,
-  file.file_type AS file_type,
-  file.file_description AS file_description,
-  file.file_size AS file_size,
-  file.md5sum AS md5sum,
-  st.study_id AS study_id,
-  st.phs_accession as phs_accession,
-  st.study_acronym as study_acronym,
-  st.study_short_title as study_short_title,
-  p.participant_id AS participant_id,
-  null AS sample_id,
-  null as combined_filters,
-  COLLECT(DISTINCT {
-      race: races,
-      sex_at_birth: p.sex_at_birth,
-      ethnicity: ethnicities
-  }) AS participant_filters,
-  COLLECT(DISTINCT {
-      age_at_diagnosis: dg.age_at_diagnosis,
-      diagnosis_anatomic_site: dg.anatomic_site,
-      disease_phase: dg.disease_phase,
-      diagnosis_classification_system: dg.diagnosis_classification_system,
-      diagnosis_verification_status: dg.diagnosis_verification_status,
-      diagnosis_basis: dg.diagnosis_basis,
-      diagnosis_comment: dg.diagnosis_comment,
-      diagnosis_classification: dg.diagnosis_classification
-  }) AS diagnosis_filters,
-  COLLECT(DISTINCT fu.vital_status) as vital_status,
-  COLLECT(DISTINCT {
-      sample_anatomic_site: sm.anatomic_site,
-      participant_age_at_collection: sm.participant_age_at_collection,
-      sample_tumor_status: sm.sample_tumor_status,
-      tumor_classification: sm.tumor_classification
-  }) AS sample_filters,
-  COLLECT(DISTINCT stf.grant_id) as grant_id,
-  COLLECT(DISTINCT stp.institution) as institution,
-  null AS library_selection,
-  null AS library_source,
-  null AS library_strategy
-UNION ALL
-with st
-MATCH (file:single_cell_sequencing_file)
-MATCH (p:participant)&lt;-[:of_sample]-(sm1:sample)&lt;-[*0..2]-(sm:sample)&lt;-[:of_single_cell_sequencing_file]-(file)
-MATCH (st)&lt;-[:of_participant]-(p)
-OPTIONAL MATCH (st)&lt;-[:of_publication]-(pub:publication)
-OPTIONAL MATCH (p)&lt;-[:of_diagnosis]-(dg:diagnosis)
-OPTIONAL MATCH (p)&lt;-[:of_follow_up]-(fu:follow_up)
-OPTIONAL MATCH (st)&lt;-[:of_study_personnel]-(stp:study_personnel)
-OPTIONAL MATCH (st)&lt;-[:of_study_funding]-(stf:study_funding)
-UNWIND apoc.text.split(p.ethnicity, ';') AS ethnicities
-UNWIND apoc.text.split(p.race, ';') AS races
-with file, p, sm1, sm, st, ethnicities, races, fu, dg, stf, stp
-RETURN DISTINCT
-  file.id as id,
-  p.id as pid,
-  file.single_cell_sequencing_file_id AS file_id,
-  file.dcf_indexd_guid AS guid,
-  file.file_name AS file_name,
-  'Single Cell Sequencing' AS file_category,
-  file.file_type AS file_type,
-  file.file_description AS file_description,
-  file.file_size AS file_size,
-  file.md5sum AS md5sum,
-  st.study_id AS study_id,
-  st.phs_accession as phs_accession,
-  st.study_acronym as study_acronym,
-  st.study_short_title as study_short_title,
-  p.participant_id AS participant_id,
-  CASE sm1.sample_id WHEN sm.sample_id THEN sm.sample_id
-            ELSE sm1.sample_id + ',' + sm.sample_id END AS sample_id,
-  null as combined_filters,
-  COLLECT(DISTINCT {
-      race: races,
-      sex_at_birth: p.sex_at_birth,
-      ethnicity: ethnicities
-  }) AS participant_filters,
-  COLLECT(DISTINCT {
-      age_at_diagnosis: dg.age_at_diagnosis,
-      diagnosis_anatomic_site: dg.anatomic_site,
-      disease_phase: dg.disease_phase,
-      diagnosis_classification_system: dg.diagnosis_classification_system,
-      diagnosis_verification_status: dg.diagnosis_verification_status,
-      diagnosis_basis: dg.diagnosis_basis,
-      diagnosis_comment: dg.diagnosis_comment,
-      diagnosis_classification: dg.diagnosis_classification
-  }) AS diagnosis_filters,
-  COLLECT(DISTINCT fu.vital_status) as vital_status,
-  CASE sm1.sample_id WHEN sm.sample_id THEN COLLECT(DISTINCT {
-                              sample_anatomic_site: sm.anatomic_site,
-                              participant_age_at_collection: sm.participant_age_at_collection,
-                              sample_tumor_status: sm.sample_tumor_status,
-                              tumor_classification: sm.tumor_classification
-                          })
-            ELSE apoc.coll.union(COLLECT(DISTINCT {
-                              sample_anatomic_site: sm1.anatomic_site,
-                              participant_age_at_collection: sm1.participant_age_at_collection,
-                              sample_tumor_status: sm1.sample_tumor_status,
-                              tumor_classification: sm1.tumor_classification
-                          }), COLLECT(DISTINCT {
-                              sample_anatomic_site: sm.anatomic_site,
-                              participant_age_at_collection: sm.participant_age_at_collection,
-                              sample_tumor_status: sm.sample_tumor_status,
-                              tumor_classification: sm.tumor_classification
-                          })) END AS sample_filters,
-  COLLECT(DISTINCT stf.grant_id) as grant_id,
-  COLLECT(DISTINCT stp.institution) as institution,
-  file.library_selection AS library_selection,
-  file.library_source AS library_source,
-  file.library_strategy AS library_strategy
-UNION ALL
-with st
-MATCH (file:sequencing_file)
-MATCH (p:participant)&lt;-[:of_sample]-(sm1:sample)&lt;-[*0..2]-(sm:sample)&lt;-[:of_sequencing_file]-(file)
-MATCH (st)&lt;-[:of_participant]-(p)
-OPTIONAL MATCH (st)&lt;-[:of_publication]-(pub:publication)
-OPTIONAL MATCH (p)&lt;-[:of_diagnosis]-(dg:diagnosis)
-OPTIONAL MATCH (p)&lt;-[:of_follow_up]-(fu:follow_up)
-OPTIONAL MATCH (st)&lt;-[:of_study_personnel]-(stp:study_personnel)
-OPTIONAL MATCH (st)&lt;-[:of_study_funding]-(stf:study_funding)
-UNWIND apoc.text.split(p.ethnicity, ';') AS ethnicities
-UNWIND apoc.text.split(p.race, ';') AS races
-with file, p, sm1, sm, st, ethnicities, races, fu, dg, stf, stp
-RETURN DISTINCT
-  file.id as id,
-  p.id as pid,
-  file.sequencing_file_id AS file_id,
-  file.dcf_indexd_guid AS guid,
-  file.file_name AS file_name,
-  'Sequencing' AS file_category,
-  file.file_type AS file_type,
-  file.file_description AS file_description,
-  file.file_size AS file_size,
-  file.md5sum AS md5sum,
-  st.study_id AS study_id,
-  st.phs_accession as phs_accession,
-  st.study_acronym as study_acronym,
-  st.study_short_title as study_short_title,
-  p.participant_id AS participant_id,
-  CASE sm1.sample_id WHEN sm.sample_id THEN sm.sample_id
-            ELSE sm1.sample_id + ',' + sm.sample_id END AS sample_id,
-  null as combined_filters,
-  COLLECT(DISTINCT {
-      race: races,
-      sex_at_birth: p.sex_at_birth,
-      ethnicity: ethnicities
-  }) AS participant_filters,
-  COLLECT(DISTINCT {
-      age_at_diagnosis: dg.age_at_diagnosis,
-      diagnosis_anatomic_site: dg.anatomic_site,
-      disease_phase: dg.disease_phase,
-      diagnosis_classification_system: dg.diagnosis_classification_system,
-      diagnosis_verification_status: dg.diagnosis_verification_status,
-      diagnosis_basis: dg.diagnosis_basis,
-      diagnosis_comment: dg.diagnosis_comment,
-      diagnosis_classification: dg.diagnosis_classification
-  }) AS diagnosis_filters,
-  COLLECT(DISTINCT fu.vital_status) as vital_status,
-  CASE sm1.sample_id WHEN sm.sample_id THEN COLLECT(DISTINCT {
-                              sample_anatomic_site: sm.anatomic_site,
-                              participant_age_at_collection: sm.participant_age_at_collection,
-                              sample_tumor_status: sm.sample_tumor_status,
-                              tumor_classification: sm.tumor_classification
-                          })
-            ELSE apoc.coll.union(COLLECT(DISTINCT {
-                              sample_anatomic_site: sm1.anatomic_site,
-                              participant_age_at_collection: sm1.participant_age_at_collection,
-                              sample_tumor_status: sm1.sample_tumor_status,
-                              tumor_classification: sm1.tumor_classification
-                          }), COLLECT(DISTINCT {
-                              sample_anatomic_site: sm.anatomic_site,
-                              participant_age_at_collection: sm.participant_age_at_collection,
-                              sample_tumor_status: sm.sample_tumor_status,
-                              tumor_classification: sm.tumor_classification
-                          })) END AS sample_filters,
-  COLLECT(DISTINCT stf.grant_id) as grant_id,
-  COLLECT(DISTINCT stp.institution) as institution,
-  file.library_selection AS library_selection,
-  file.library_source AS library_source,
-  file.library_strategy AS library_strategy
-UNION ALL
-with st
-MATCH (file:cytogenomic_file)
-MATCH (p:participant)&lt;-[:of_sample]-(sm1:sample)&lt;-[*0..2]-(sm:sample)&lt;-[:of_cytogenomic_file]-(file)
-MATCH (st)&lt;-[:of_participant]-(p)
-OPTIONAL MATCH (st)&lt;-[:of_publication]-(pub:publication)
-OPTIONAL MATCH (p)&lt;-[:of_diagnosis]-(dg:diagnosis)
-OPTIONAL MATCH (p)&lt;-[:of_follow_up]-(fu:follow_up)
-OPTIONAL MATCH (st)&lt;-[:of_study_personnel]-(stp:study_personnel)
-OPTIONAL MATCH (st)&lt;-[:of_study_funding]-(stf:study_funding)
-UNWIND apoc.text.split(p.ethnicity, ';') AS ethnicities
-UNWIND apoc.text.split(p.race, ';') AS races
-with file, p, sm1, sm, st, ethnicities, races, fu, dg, stf, stp
-RETURN DISTINCT
-  file.id as id,
-  p.id as pid,
-  file.cytogenomic_file_id AS file_id,
-  file.dcf_indexd_guid AS guid,
-  file.file_name AS file_name,
-  'Cytogenomic' AS file_category,
-  file.file_type AS file_type,
-  file.file_description AS file_description,
-  file.file_size AS file_size,
-  file.md5sum AS md5sum,
-  st.study_id AS study_id,
-  st.phs_accession as phs_accession,
-  st.study_acronym as study_acronym,
-  st.study_short_title as study_short_title,
-  p.participant_id AS participant_id,
-  CASE sm1.sample_id WHEN sm.sample_id THEN sm.sample_id
-            ELSE sm1.sample_id + ',' + sm.sample_id END AS sample_id,
-  null as combined_filters,
-  COLLECT(DISTINCT {
-      race: races,
-      sex_at_birth: p.sex_at_birth,
-      ethnicity: ethnicities
-  }) AS participant_filters,
-  COLLECT(DISTINCT {
-      age_at_diagnosis: dg.age_at_diagnosis,
-      diagnosis_anatomic_site: dg.anatomic_site,
-      disease_phase: dg.disease_phase,
-      diagnosis_classification_system: dg.diagnosis_classification_system,
-      diagnosis_verification_status: dg.diagnosis_verification_status,
-      diagnosis_basis: dg.diagnosis_basis,
-      diagnosis_comment: dg.diagnosis_comment,
-      diagnosis_classification: dg.diagnosis_classification
-  }) AS diagnosis_filters,
-  COLLECT(DISTINCT fu.vital_status) as vital_status,
-  CASE sm1.sample_id WHEN sm.sample_id THEN COLLECT(DISTINCT {
-                              sample_anatomic_site: sm.anatomic_site,
-                              participant_age_at_collection: sm.participant_age_at_collection,
-                              sample_tumor_status: sm.sample_tumor_status,
-                              tumor_classification: sm.tumor_classification
-                          })
-            ELSE apoc.coll.union(COLLECT(DISTINCT {
-                              sample_anatomic_site: sm1.anatomic_site,
-                              participant_age_at_collection: sm1.participant_age_at_collection,
-                              sample_tumor_status: sm1.sample_tumor_status,
-                              tumor_classification: sm1.tumor_classification
-                          }), COLLECT(DISTINCT {
-                              sample_anatomic_site: sm.anatomic_site,
-                              participant_age_at_collection: sm.participant_age_at_collection,
-                              sample_tumor_status: sm.sample_tumor_status,
-                              tumor_classification: sm.tumor_classification
-                          })) END AS sample_filters,
-  COLLECT(DISTINCT stf.grant_id) as grant_id,
-  COLLECT(DISTINCT stp.institution) as institution,
-  null AS library_selection,
-  null AS library_source,
-  null AS library_strategy
-UNION ALL
-with st
-MATCH (file)
-WHERE (file:sequencing_file OR file:pathology_file OR file:methylation_array_file OR file:single_cell_sequencing_file OR file:cytogenomic_file)
-MATCH (st)&lt;-[:of_cell_line|of_pdx]-(cl)&lt;--(sm:sample)
-Where (cl: cell_line or cl: pdx)
-MATCH (sm)&lt;--(file)
-OPTIONAL MATCH (st)&lt;-[:of_publication]-(pub:publication)
-OPTIONAL MATCH (st)&lt;--(p:participant)&lt;-[:of_diagnosis]-(dg:diagnosis)
-OPTIONAL MATCH (st)&lt;--(p)&lt;-[:of_follow_up]-(fu:follow_up)
-OPTIONAL MATCH (st)&lt;-[:of_study_personnel]-(stp:study_personnel)
-OPTIONAL MATCH (st)&lt;-[:of_study_funding]-(stf:study_funding)
-with file, sm, st, fu, dg, stf, stp
-RETURN DISTINCT
-  file.id as id,
-  null as pid,
-  CASE LABELS(file)[0]
-        WHEN 'sequencing_file' THEN file.sequencing_file_id
-        WHEN 'single_cell_sequencing_file' THEN file.single_cell_sequencing_file_id
-        WHEN 'cytogenomic_file' THEN file.cytogenomic_file_id
-        WHEN 'pathology_file' THEN file.pathology_file_id
-        WHEN 'methylation_array_file' THEN file.methylation_array_file_id END AS file_id,
-  file.dcf_indexd_guid AS guid,
-  file.file_name AS file_name,
-  CASE LABELS(file)[0]
-        WHEN 'sequencing_file' THEN 'Sequencing'
-        WHEN 'single_cell_sequencing_file' THEN 'Single Cell Sequencing'
-        WHEN 'cytogenomic_file' THEN 'Cytogenomic'
-        WHEN 'pathology_file' THEN 'Pathology imaging'
-        WHEN 'methylation_array_file' THEN 'Methylation array' END AS file_category,
-  file.file_type AS file_type,
-  file.file_description AS file_description,
-  file.file_size AS file_size,
-  file.md5sum AS md5sum,
-  st.study_id AS study_id,
-  st.phs_accession as phs_accession,
-  st.study_acronym as study_acronym,
-  st.study_short_title as study_short_title,
-  null AS participant_id,
-  sm.sample_id AS sample_id,
-  null as combined_filters,
-  null AS participant_filters,
-  COLLECT(DISTINCT {
-      age_at_diagnosis: dg.age_at_diagnosis,
-      diagnosis_anatomic_site: dg.anatomic_site,
-      disease_phase: dg.disease_phase,
-      diagnosis_classification_system: dg.diagnosis_classification_system,
-      diagnosis_verification_status: dg.diagnosis_verification_status,
-      diagnosis_basis: dg.diagnosis_basis,
-      diagnosis_comment: dg.diagnosis_comment,
-      diagnosis_classification: dg.diagnosis_classification
-  }) AS diagnosis_filters,
-  COLLECT(DISTINCT fu.vital_status) as vital_status,
-  COLLECT(DISTINCT {
-      sample_anatomic_site: sm.anatomic_site,
-      participant_age_at_collection: sm.participant_age_at_collection,
-      sample_tumor_status: sm.sample_tumor_status,
-      tumor_classification: sm.tumor_classification
-  }) AS sample_filters,
-  COLLECT(DISTINCT stf.grant_id) as grant_id,
-  COLLECT(DISTINCT stp.institution) as institution,
-  CASE LABELS(file)[0]
-            WHEN 'sequencing_file' THEN file.library_selection
-            WHEN 'single_cell_sequencing_file' THEN file.library_selection
-            ELSE null END AS library_selection,
-  CASE LABELS(file)[0]
-            WHEN 'sequencing_file' THEN file.library_source
-            WHEN 'single_cell_sequencing_file' THEN file.library_source
-            ELSE null END AS library_source,
-  CASE LABELS(file)[0]
-            WHEN 'sequencing_file' THEN file.library_strategy
-            WHEN 'single_cell_sequencing_file' THEN file.library_strategy
-            ELSE null END AS library_strategy
-}
-with id, guid, file_name, file_category, file_type, file_description, file_size, md5sum, study_id, phs_accession, study_acronym, study_short_title, participant_id, sample_id, participant_filters,diagnosis_filters, vital_status, sample_filters, grant_id, institution,library_selection,library_source,library_strategy
-unwind participant_filters as participant_filter
-with id, guid, file_name, file_category, file_type, file_description, file_size, md5sum, study_id, phs_accession, study_acronym, study_short_title, participant_id, sample_id, participant_filter,diagnosis_filters, vital_status, sample_filters, grant_id, institution,library_selection,library_source,library_strategy
- unwind diagnosis_filters as diagnosis_filter
-with id, guid, file_name, file_category, file_type, file_description, file_size, md5sum, study_id, phs_accession, study_acronym, study_short_title, participant_id, sample_id,diagnosis_filter, vital_status, sample_filters, grant_id, institution,library_selection,library_source,library_strategy
- with id, guid, file_name, file_category, file_type, file_description, file_size, md5sum, study_id, phs_accession, study_acronym, study_short_title, participant_id, sample_id, vital_status, sample_filters, grant_id, institution,library_selection,library_source,library_strategy
- unwind sample_filters as sample_filter
-with id, guid, file_name, file_category, file_type, file_description, file_size, md5sum, study_id, phs_accession, study_acronym, study_short_title, participant_id, sample_id, sample_filter, grant_id, institution,library_selection,library_source,library_strategy
- with distinct id, guid, file_name, file_category, file_type, file_description, file_size, md5sum, study_id, phs_accession, study_acronym, study_short_title, participant_id, sample_id, grant_id, institution,library_selection,library_source,library_strategy
-call {
-  with id, guid, file_name, file_category, file_type, file_description, file_size, md5sum, study_id, phs_accession, study_acronym, study_short_title, participant_id, sample_id, grant_id, institution,library_selection,library_source,library_strategy
-  return id as fid, guid as dig, file_name as fn, file_category as fc, file_type as ft, file_description as fd, file_size as fsize, md5sum as md5, study_id as sid, phs_accession as pa, study_acronym as sa, study_short_title as sst, participant_id as pid, sample_id as smid, grant_id as gid, institution as istt,library_selection as ls,library_source as lis,library_strategy as listr
-  UNION ALL
-  with study_id
-  MATCH (file:clinical_measure_file)
-  MATCH (stu:study)&lt;-[:of_clinical_measure_file]-(file)
-  where stu.study_id = study_id
-  OPTIONAL MATCH (stu)&lt;-[:of_study_personnel]-(stp:study_personnel)
-  OPTIONAL MATCH (stu)&lt;-[:of_study_funding]-(stf:study_funding)
-  With file, stu, stf, stp
-  RETURN DISTINCT
-    file.id as fid,
-    file.dcf_indexd_guid AS dig,
-    file.file_name AS fn,
-    'Clinical data' AS fc,
-    file.file_type AS ft,
-    file.file_description AS fd,
-    file.file_size AS fsize,
-    file.md5sum AS md5,
-    stu.study_id AS sid,
-    stu.phs_accession as pa,
-    stu.study_acronym as sa,
-    stu.study_short_title as sst,
-    null AS pid,
-    null AS smid,
-    COLLECT(DISTINCT stf.grant_id) as gid,
-    COLLECT(DISTINCT stp.institution) as istt,
-    null AS ls,
-    null AS lis,
-    null AS listr
-}
-with fid as id, dig as guid, fn as file_name, fc as file_category, ft as file_type, fd as file_description, fsize as file_size, md5 as md5sum, sid as study_id, pa as phs_accession, sa as study_acronym, sst as study_short_title, pid as participant_id, smid as sample_id, gid as grant_id, istt as institution,ls as library_selection,lis as library_source,listr as library_strategy
-where  ANY(element IN ['University of Southern California']  with st WHERE element IN institution)  and library_selection in ['Unspecified']  
-with id, guid, file_name, file_category, file_type, file_description, file_size, ['Bytes', 'KB', 'MB', 'GB', 'TB'] AS units,
-        toInteger(floor(log(file_size)/log(1024))) as i,
-        2 as precision, md5sum, study_id, phs_accession, study_acronym, study_short_title, participant_id, sample_id, grant_id, institution,library_selection,library_source,library_strategy
-with id, guid, file_name, file_category, file_type, file_description, file_size, file_size /(1024^i) AS value,
-        10^precision AS factor,
-        units[i] as unit, md5sum, study_id, phs_accession, study_acronym, study_short_title, participant_id, sample_id, grant_id, institution,library_selection,library_source,library_strategy
-with id, guid, file_name, file_category, file_type, file_description, unit,
-        round(factor * value)/factor AS size, md5sum, study_id, phs_accession, study_acronym, study_short_title, participant_id, sample_id, grant_id, institution,library_selection,library_source,library_strategy     
-with DISTINCT id,
-        file_name,
-        file_category,
-        file_description,
-        file_type,
-        CASE size % 1 WHEN 0 THEN apoc.convert.toInteger(size)+' ' +unit ELSE size+' ' +unit END AS file_size_new,
-        study_id,
-        participant_id,
-        sample_id,
-        guid,
-        md5sum
-RETURN file_name AS `File Name`,
-file_category As `File Category`,
-file_description As `File Description`,
-file_type As `File Type`,
-file_size_new As `File Size`,
-study_id As `Study ID`,
-coalesce(participant_id, '') As `Participant ID`,
-coalesce(sample_id, '') As `Sample ID`,
-guid As `GUID`,
-md5sum As `MD5Sum`
-ORDER BY file_name LIMIT 100</t>
   </si>
   <si>
     <t>TC08_CCDI_PHS-Accession-phs002620_Institution-NCI_LibSelec-PolyA_Neo4jData.xlsx</t>
@@ -2030,6 +1412,625 @@
           sample_tumor_status as `Sample Tumor Status`,
           tumor_classification as `Sample Tumor Classification`
 Order by sample_id Limit 100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Match (st:study)
+where st.phs_accession in ['phs002620']  
+with st
+Call {
+with st 
+MATCH (file:clinical_measure_file)
+MATCH (p:participant)-[:of_clinical_measure_file]-(file)
+MATCH (st)&lt;-[:of_participant]-(p)
+OPTIONAL MATCH (p)&lt;-[:of_sample]-(sm:sample)
+OPTIONAL MATCH (st)&lt;-[:of_publication]-(pub:publication)
+OPTIONAL MATCH (p)&lt;-[:of_diagnosis]-(dg:diagnosis)
+OPTIONAL MATCH (p)&lt;-[:of_follow_up]-(fu:follow_up)
+OPTIONAL MATCH (st)&lt;-[:of_study_personnel]-(stp:study_personnel)
+OPTIONAL MATCH (st)&lt;-[:of_study_funding]-(stf:study_funding)
+UNWIND apoc.text.split(p.ethnicity, ';') AS ethnicities
+UNWIND apoc.text.split(p.race, ';') AS races
+RETURN DISTINCT
+  file.id as id,
+  p.id as pid,
+  file.clinical_measure_file_id AS file_id,
+  file.dcf_indexd_guid AS guid,
+  file.file_name AS file_name,
+  'Clinical data' AS file_category,
+  file.file_type AS file_type,
+  file.file_description AS file_description,
+  file.file_size AS file_size,
+  file.md5sum AS md5sum,
+  st.study_id AS study_id,
+  st.phs_accession as phs_accession,
+  st.study_acronym as study_acronym,
+  st.study_short_title as study_short_title,
+  p.participant_id AS participant_id,
+  null AS sample_id,
+  null as combined_filters,
+  COLLECT(DISTINCT {
+      race: races,
+      sex_at_birth: p.sex_at_birth,
+      ethnicity: ethnicities
+  }) AS participant_filters,
+  COLLECT(DISTINCT {
+      age_at_diagnosis: dg.age_at_diagnosis,
+      diagnosis_anatomic_site: dg.anatomic_site,
+      disease_phase: dg.disease_phase,
+      diagnosis_classification_system: dg.diagnosis_classification_system,
+      diagnosis_verification_status: dg.diagnosis_verification_status,
+      diagnosis_basis: dg.diagnosis_basis,
+      diagnosis_comment: dg.diagnosis_comment,
+      diagnosis_classification: dg.diagnosis_classification
+  }) AS diagnosis_filters,
+  COLLECT(DISTINCT fu.vital_status) as vital_status,
+  COLLECT(DISTINCT {
+      sample_anatomic_site: sm.anatomic_site,
+      participant_age_at_collection: sm.participant_age_at_collection,
+      sample_tumor_status: sm.sample_tumor_status,
+      tumor_classification: sm.tumor_classification
+  }) AS sample_filters,
+  COLLECT(DISTINCT stf.grant_id) as grant_id,
+  COLLECT(DISTINCT stp.institution) as institution,      
+  null AS library_selection,
+  null AS library_source,
+  null AS library_strategy
+UNION ALL
+with st
+MATCH (file:methylation_array_file)
+MATCH (p:participant)&lt;-[:of_sample]-(sm1:sample)&lt;-[*0..2]-(sm:sample)&lt;-[:of_methylation_array_file]-(file)
+MATCH (st)&lt;-[:of_participant]-(p)
+OPTIONAL MATCH (st)&lt;-[:of_publication]-(pub:publication)
+OPTIONAL MATCH (p)&lt;-[:of_diagnosis]-(dg:diagnosis)
+OPTIONAL MATCH (p)&lt;-[:of_follow_up]-(fu:follow_up)
+OPTIONAL MATCH (st)&lt;-[:of_study_personnel]-(stp:study_personnel)
+OPTIONAL MATCH (st)&lt;-[:of_study_funding]-(stf:study_funding)
+UNWIND apoc.text.split(p.ethnicity, ';') AS ethnicities
+UNWIND apoc.text.split(p.race, ';') AS races
+with file, p, sm1, sm, st, ethnicities, races, fu, dg, stf, stp
+RETURN DISTINCT
+  file.id as id,
+  p.id as pid,
+  file.methylation_array_file_id AS file_id,
+  file.dcf_indexd_guid AS guid,
+  file.file_name AS file_name,
+  'Methylation array' AS file_category,
+  file.file_type AS file_type,
+  file.file_description AS file_description,
+  file.file_size AS file_size,
+  file.md5sum AS md5sum,
+  st.study_id AS study_id,
+  st.phs_accession as phs_accession,
+  st.study_acronym as study_acronym,
+  st.study_short_title as study_short_title,
+  p.participant_id AS participant_id,
+  CASE sm1.sample_id WHEN sm.sample_id THEN sm.sample_id
+            ELSE sm1.sample_id + ',' + sm.sample_id END AS sample_id,
+  null as combined_filters,
+  COLLECT(DISTINCT {
+      race: races,
+      sex_at_birth: p.sex_at_birth,
+      ethnicity: ethnicities
+  }) AS participant_filters,
+  COLLECT(DISTINCT {
+      age_at_diagnosis: dg.age_at_diagnosis,
+      diagnosis_anatomic_site: dg.anatomic_site,
+      disease_phase: dg.disease_phase,
+      diagnosis_classification_system: dg.diagnosis_classification_system,
+      diagnosis_verification_status: dg.diagnosis_verification_status,
+      diagnosis_basis: dg.diagnosis_basis,
+      diagnosis_comment: dg.diagnosis_comment,
+      diagnosis_classification: dg.diagnosis_classification
+  }) AS diagnosis_filters,
+  COLLECT(DISTINCT fu.vital_status) as vital_status,
+  CASE sm1.sample_id WHEN sm.sample_id THEN COLLECT(DISTINCT {
+                              sample_anatomic_site: sm.anatomic_site,
+                              participant_age_at_collection: sm.participant_age_at_collection,
+                              sample_tumor_status: sm.sample_tumor_status,
+                              tumor_classification: sm.tumor_classification
+                          })
+            ELSE apoc.coll.union(COLLECT(DISTINCT {
+                              sample_anatomic_site: sm1.anatomic_site,
+                              participant_age_at_collection: sm1.participant_age_at_collection,
+                              sample_tumor_status: sm1.sample_tumor_status,
+                              tumor_classification: sm1.tumor_classification
+                          }), COLLECT(DISTINCT {
+                              sample_anatomic_site: sm.anatomic_site,
+                              participant_age_at_collection: sm.participant_age_at_collection,
+                              sample_tumor_status: sm.sample_tumor_status,
+                              tumor_classification: sm.tumor_classification
+                          })) END AS sample_filters,
+  COLLECT(DISTINCT stf.grant_id) as grant_id,
+  COLLECT(DISTINCT stp.institution) as institution,
+  null AS library_selection,
+  null AS library_source,
+  null AS library_strategy
+UNION ALL
+with st
+MATCH (file:pathology_file)
+MATCH (p:participant)&lt;-[:of_sample]-(sm1:sample)&lt;-[*0..2]-(sm:sample)&lt;-[:of_pathology_file]-(file)
+MATCH (st)&lt;-[:of_participant]-(p)
+OPTIONAL MATCH (st)&lt;-[:of_publication]-(pub:publication)
+OPTIONAL MATCH (p)&lt;-[:of_diagnosis]-(dg:diagnosis)
+OPTIONAL MATCH (p)&lt;-[:of_follow_up]-(fu:follow_up)
+OPTIONAL MATCH (st)&lt;-[:of_study_personnel]-(stp:study_personnel)
+OPTIONAL MATCH (st)&lt;-[:of_study_funding]-(stf:study_funding)
+UNWIND apoc.text.split(p.ethnicity, ';') AS ethnicities
+UNWIND apoc.text.split(p.race, ';') AS races
+with file, p, sm1, sm, st, ethnicities, races, fu, dg, stf, stp
+RETURN DISTINCT
+  file.id as id,
+  p.id as pid,
+  file.pathology_file_id AS file_id,
+  file.dcf_indexd_guid AS guid,
+  file.file_name AS file_name,
+  'Pathology imaging' AS file_category,
+  file.file_type AS file_type,
+  file.file_description AS file_description,
+  file.file_size AS file_size,
+  file.md5sum AS md5sum,
+  st.study_id AS study_id,
+  st.phs_accession as phs_accession,
+  st.study_acronym as study_acronym,
+  st.study_short_title as study_short_title,
+  p.participant_id AS participant_id,
+  CASE sm1.sample_id WHEN sm.sample_id THEN sm.sample_id
+            ELSE sm1.sample_id + ',' + sm.sample_id END AS sample_id,
+  null as combined_filters,
+  COLLECT(DISTINCT {
+      race: races,
+      sex_at_birth: p.sex_at_birth,
+      ethnicity: ethnicities
+  }) AS participant_filters,
+  COLLECT(DISTINCT {
+      age_at_diagnosis: dg.age_at_diagnosis,
+      diagnosis_anatomic_site: dg.anatomic_site,
+      disease_phase: dg.disease_phase,
+      diagnosis_classification_system: dg.diagnosis_classification_system,
+      diagnosis_verification_status: dg.diagnosis_verification_status,
+      diagnosis_basis: dg.diagnosis_basis,
+      diagnosis_comment: dg.diagnosis_comment,
+      diagnosis_classification: dg.diagnosis_classification
+  }) AS diagnosis_filters,
+  COLLECT(DISTINCT fu.vital_status) as vital_status,
+  CASE sm1.sample_id WHEN sm.sample_id THEN COLLECT(DISTINCT {
+                              sample_anatomic_site: sm.anatomic_site,
+                              participant_age_at_collection: sm.participant_age_at_collection,
+                              sample_tumor_status: sm.sample_tumor_status,
+                              tumor_classification: sm.tumor_classification
+                          })
+            ELSE apoc.coll.union(COLLECT(DISTINCT {
+                              sample_anatomic_site: sm1.anatomic_site,
+                              participant_age_at_collection: sm1.participant_age_at_collection,
+                              sample_tumor_status: sm1.sample_tumor_status,
+                              tumor_classification: sm1.tumor_classification
+                          }), COLLECT(DISTINCT {
+                              sample_anatomic_site: sm.anatomic_site,
+                              participant_age_at_collection: sm.participant_age_at_collection,
+                              sample_tumor_status: sm.sample_tumor_status,
+                              tumor_classification: sm.tumor_classification
+                          })) END AS sample_filters,
+  COLLECT(DISTINCT stf.grant_id) as grant_id,
+  COLLECT(DISTINCT stp.institution) as institution,
+  file.library_selection AS library_selection,
+  file.library_source AS library_source,
+  file.library_strategy AS library_strategy
+UNION ALL
+with st
+MATCH (file:radiology_file)
+MATCH (p:participant)&lt;-[:of_radiology_file]-(file)
+MATCH (st)&lt;-[:of_participant]-(p)
+OPTIONAL MATCH (p)&lt;-[:of_sample]-(sm:sample)
+OPTIONAL MATCH (st)&lt;-[:of_publication]-(pub:publication)
+OPTIONAL MATCH (p)&lt;-[:of_diagnosis]-(dg:diagnosis)
+OPTIONAL MATCH (p)&lt;-[:of_follow_up]-(fu:follow_up)
+OPTIONAL MATCH (st)&lt;-[:of_study_personnel]-(stp:study_personnel)
+OPTIONAL MATCH (st)&lt;-[:of_study_funding]-(stf:study_funding)
+UNWIND apoc.text.split(p.ethnicity, ';') AS ethnicities
+UNWIND apoc.text.split(p.race, ';') AS races
+RETURN DISTINCT
+  file.id as id,
+  p.id as pid,
+  file.radiology_file_id AS file_id,
+  file.dcf_indexd_guid AS guid,
+  file.file_name AS file_name,
+  'Radiology imaging' AS file_category,
+  file.file_type AS file_type,
+  file.file_description AS file_description,
+  file.file_size AS file_size,
+  file.md5sum AS md5sum,
+  st.study_id AS study_id,
+  st.phs_accession as phs_accession,
+  st.study_acronym as study_acronym,
+  st.study_short_title as study_short_title,
+  p.participant_id AS participant_id,
+  null AS sample_id,
+  null as combined_filters,
+  COLLECT(DISTINCT {
+      race: races,
+      sex_at_birth: p.sex_at_birth,
+      ethnicity: ethnicities
+  }) AS participant_filters,
+  COLLECT(DISTINCT {
+      age_at_diagnosis: dg.age_at_diagnosis,
+      diagnosis_anatomic_site: dg.anatomic_site,
+      disease_phase: dg.disease_phase,
+      diagnosis_classification_system: dg.diagnosis_classification_system,
+      diagnosis_verification_status: dg.diagnosis_verification_status,
+      diagnosis_basis: dg.diagnosis_basis,
+      diagnosis_comment: dg.diagnosis_comment,
+      diagnosis_classification: dg.diagnosis_classification
+  }) AS diagnosis_filters,
+  COLLECT(DISTINCT fu.vital_status) as vital_status,
+  COLLECT(DISTINCT {
+      sample_anatomic_site: sm.anatomic_site,
+      participant_age_at_collection: sm.participant_age_at_collection,
+      sample_tumor_status: sm.sample_tumor_status,
+      tumor_classification: sm.tumor_classification
+  }) AS sample_filters,
+  COLLECT(DISTINCT stf.grant_id) as grant_id,
+  COLLECT(DISTINCT stp.institution) as institution,
+  null AS library_selection,
+  null AS library_source,
+  null AS library_strategy
+UNION ALL
+with st
+MATCH (file:single_cell_sequencing_file)
+MATCH (p:participant)&lt;-[:of_sample]-(sm1:sample)&lt;-[*0..2]-(sm:sample)&lt;-[:of_single_cell_sequencing_file]-(file)
+MATCH (st)&lt;-[:of_participant]-(p)
+OPTIONAL MATCH (st)&lt;-[:of_publication]-(pub:publication)
+OPTIONAL MATCH (p)&lt;-[:of_diagnosis]-(dg:diagnosis)
+OPTIONAL MATCH (p)&lt;-[:of_follow_up]-(fu:follow_up)
+OPTIONAL MATCH (st)&lt;-[:of_study_personnel]-(stp:study_personnel)
+OPTIONAL MATCH (st)&lt;-[:of_study_funding]-(stf:study_funding)
+UNWIND apoc.text.split(p.ethnicity, ';') AS ethnicities
+UNWIND apoc.text.split(p.race, ';') AS races
+with file, p, sm1, sm, st, ethnicities, races, fu, dg, stf, stp
+RETURN DISTINCT
+  file.id as id,
+  p.id as pid,
+  file.single_cell_sequencing_file_id AS file_id,
+  file.dcf_indexd_guid AS guid,
+  file.file_name AS file_name,
+  'Single Cell Sequencing' AS file_category,
+  file.file_type AS file_type,
+  file.file_description AS file_description,
+  file.file_size AS file_size,
+  file.md5sum AS md5sum,
+  st.study_id AS study_id,
+  st.phs_accession as phs_accession,
+  st.study_acronym as study_acronym,
+  st.study_short_title as study_short_title,
+  p.participant_id AS participant_id,
+  CASE sm1.sample_id WHEN sm.sample_id THEN sm.sample_id
+            ELSE sm1.sample_id + ',' + sm.sample_id END AS sample_id,
+  null as combined_filters,
+  COLLECT(DISTINCT {
+      race: races,
+      sex_at_birth: p.sex_at_birth,
+      ethnicity: ethnicities
+  }) AS participant_filters,
+  COLLECT(DISTINCT {
+      age_at_diagnosis: dg.age_at_diagnosis,
+      diagnosis_anatomic_site: dg.anatomic_site,
+      disease_phase: dg.disease_phase,
+      diagnosis_classification_system: dg.diagnosis_classification_system,
+      diagnosis_verification_status: dg.diagnosis_verification_status,
+      diagnosis_basis: dg.diagnosis_basis,
+      diagnosis_comment: dg.diagnosis_comment,
+      diagnosis_classification: dg.diagnosis_classification
+  }) AS diagnosis_filters,
+  COLLECT(DISTINCT fu.vital_status) as vital_status,
+  CASE sm1.sample_id WHEN sm.sample_id THEN COLLECT(DISTINCT {
+                              sample_anatomic_site: sm.anatomic_site,
+                              participant_age_at_collection: sm.participant_age_at_collection,
+                              sample_tumor_status: sm.sample_tumor_status,
+                              tumor_classification: sm.tumor_classification
+                          })
+            ELSE apoc.coll.union(COLLECT(DISTINCT {
+                              sample_anatomic_site: sm1.anatomic_site,
+                              participant_age_at_collection: sm1.participant_age_at_collection,
+                              sample_tumor_status: sm1.sample_tumor_status,
+                              tumor_classification: sm1.tumor_classification
+                          }), COLLECT(DISTINCT {
+                              sample_anatomic_site: sm.anatomic_site,
+                              participant_age_at_collection: sm.participant_age_at_collection,
+                              sample_tumor_status: sm.sample_tumor_status,
+                              tumor_classification: sm.tumor_classification
+                          })) END AS sample_filters,
+  COLLECT(DISTINCT stf.grant_id) as grant_id,
+  COLLECT(DISTINCT stp.institution) as institution,
+  file.library_selection AS library_selection,
+  file.library_source AS library_source,
+  file.library_strategy AS library_strategy
+UNION ALL
+with st
+MATCH (file:sequencing_file)
+MATCH (p:participant)&lt;-[:of_sample]-(sm1:sample)&lt;-[*0..2]-(sm:sample)&lt;-[:of_sequencing_file]-(file)
+MATCH (st)&lt;-[:of_participant]-(p)
+OPTIONAL MATCH (st)&lt;-[:of_publication]-(pub:publication)
+OPTIONAL MATCH (p)&lt;-[:of_diagnosis]-(dg:diagnosis)
+OPTIONAL MATCH (p)&lt;-[:of_follow_up]-(fu:follow_up)
+OPTIONAL MATCH (st)&lt;-[:of_study_personnel]-(stp:study_personnel)
+OPTIONAL MATCH (st)&lt;-[:of_study_funding]-(stf:study_funding)
+UNWIND apoc.text.split(p.ethnicity, ';') AS ethnicities
+UNWIND apoc.text.split(p.race, ';') AS races
+with file, p, sm1, sm, st, ethnicities, races, fu, dg, stf, stp
+RETURN DISTINCT
+  file.id as id,
+  p.id as pid,
+  file.sequencing_file_id AS file_id,
+  file.dcf_indexd_guid AS guid,
+  file.file_name AS file_name,
+  'Sequencing' AS file_category,
+  file.file_type AS file_type,
+  file.file_description AS file_description,
+  file.file_size AS file_size,
+  file.md5sum AS md5sum,
+  st.study_id AS study_id,
+  st.phs_accession as phs_accession,
+  st.study_acronym as study_acronym,
+  st.study_short_title as study_short_title,
+  p.participant_id AS participant_id,
+  CASE sm1.sample_id WHEN sm.sample_id THEN sm.sample_id
+            ELSE sm1.sample_id + ',' + sm.sample_id END AS sample_id,
+  null as combined_filters,
+  COLLECT(DISTINCT {
+      race: races,
+      sex_at_birth: p.sex_at_birth,
+      ethnicity: ethnicities
+  }) AS participant_filters,
+  COLLECT(DISTINCT {
+      age_at_diagnosis: dg.age_at_diagnosis,
+      diagnosis_anatomic_site: dg.anatomic_site,
+      disease_phase: dg.disease_phase,
+      diagnosis_classification_system: dg.diagnosis_classification_system,
+      diagnosis_verification_status: dg.diagnosis_verification_status,
+      diagnosis_basis: dg.diagnosis_basis,
+      diagnosis_comment: dg.diagnosis_comment,
+      diagnosis_classification: dg.diagnosis_classification
+  }) AS diagnosis_filters,
+  COLLECT(DISTINCT fu.vital_status) as vital_status,
+  CASE sm1.sample_id WHEN sm.sample_id THEN COLLECT(DISTINCT {
+                              sample_anatomic_site: sm.anatomic_site,
+                              participant_age_at_collection: sm.participant_age_at_collection,
+                              sample_tumor_status: sm.sample_tumor_status,
+                              tumor_classification: sm.tumor_classification
+                          })
+            ELSE apoc.coll.union(COLLECT(DISTINCT {
+                              sample_anatomic_site: sm1.anatomic_site,
+                              participant_age_at_collection: sm1.participant_age_at_collection,
+                              sample_tumor_status: sm1.sample_tumor_status,
+                              tumor_classification: sm1.tumor_classification
+                          }), COLLECT(DISTINCT {
+                              sample_anatomic_site: sm.anatomic_site,
+                              participant_age_at_collection: sm.participant_age_at_collection,
+                              sample_tumor_status: sm.sample_tumor_status,
+                              tumor_classification: sm.tumor_classification
+                          })) END AS sample_filters,
+  COLLECT(DISTINCT stf.grant_id) as grant_id,
+  COLLECT(DISTINCT stp.institution) as institution,
+  file.library_selection AS library_selection,
+  file.library_source AS library_source,
+  file.library_strategy AS library_strategy
+UNION ALL
+with st
+MATCH (file:cytogenomic_file)
+MATCH (p:participant)&lt;-[:of_sample]-(sm1:sample)&lt;-[*0..2]-(sm:sample)&lt;-[:of_cytogenomic_file]-(file)
+MATCH (st)&lt;-[:of_participant]-(p)
+OPTIONAL MATCH (st)&lt;-[:of_publication]-(pub:publication)
+OPTIONAL MATCH (p)&lt;-[:of_diagnosis]-(dg:diagnosis)
+OPTIONAL MATCH (p)&lt;-[:of_follow_up]-(fu:follow_up)
+OPTIONAL MATCH (st)&lt;-[:of_study_personnel]-(stp:study_personnel)
+OPTIONAL MATCH (st)&lt;-[:of_study_funding]-(stf:study_funding)
+UNWIND apoc.text.split(p.ethnicity, ';') AS ethnicities
+UNWIND apoc.text.split(p.race, ';') AS races
+with file, p, sm1, sm, st, ethnicities, races, fu, dg, stf, stp
+RETURN DISTINCT
+  file.id as id,
+  p.id as pid,
+  file.cytogenomic_file_id AS file_id,
+  file.dcf_indexd_guid AS guid,
+  file.file_name AS file_name,
+  'Cytogenomic' AS file_category,
+  file.file_type AS file_type,
+  file.file_description AS file_description,
+  file.file_size AS file_size,
+  file.md5sum AS md5sum,
+  st.study_id AS study_id,
+  st.phs_accession as phs_accession,
+  st.study_acronym as study_acronym,
+  st.study_short_title as study_short_title,
+  p.participant_id AS participant_id,
+  CASE sm1.sample_id WHEN sm.sample_id THEN sm.sample_id
+            ELSE sm1.sample_id + ',' + sm.sample_id END AS sample_id,
+  null as combined_filters,
+  COLLECT(DISTINCT {
+      race: races,
+      sex_at_birth: p.sex_at_birth,
+      ethnicity: ethnicities
+  }) AS participant_filters,
+  COLLECT(DISTINCT {
+      age_at_diagnosis: dg.age_at_diagnosis,
+      diagnosis_anatomic_site: dg.anatomic_site,
+      disease_phase: dg.disease_phase,
+      diagnosis_classification_system: dg.diagnosis_classification_system,
+      diagnosis_verification_status: dg.diagnosis_verification_status,
+      diagnosis_basis: dg.diagnosis_basis,
+      diagnosis_comment: dg.diagnosis_comment,
+      diagnosis_classification: dg.diagnosis_classification
+  }) AS diagnosis_filters,
+  COLLECT(DISTINCT fu.vital_status) as vital_status,
+  CASE sm1.sample_id WHEN sm.sample_id THEN COLLECT(DISTINCT {
+                              sample_anatomic_site: sm.anatomic_site,
+                              participant_age_at_collection: sm.participant_age_at_collection,
+                              sample_tumor_status: sm.sample_tumor_status,
+                              tumor_classification: sm.tumor_classification
+                          })
+            ELSE apoc.coll.union(COLLECT(DISTINCT {
+                              sample_anatomic_site: sm1.anatomic_site,
+                              participant_age_at_collection: sm1.participant_age_at_collection,
+                              sample_tumor_status: sm1.sample_tumor_status,
+                              tumor_classification: sm1.tumor_classification
+                          }), COLLECT(DISTINCT {
+                              sample_anatomic_site: sm.anatomic_site,
+                              participant_age_at_collection: sm.participant_age_at_collection,
+                              sample_tumor_status: sm.sample_tumor_status,
+                              tumor_classification: sm.tumor_classification
+                          })) END AS sample_filters,
+  COLLECT(DISTINCT stf.grant_id) as grant_id,
+  COLLECT(DISTINCT stp.institution) as institution,
+  null AS library_selection,
+  null AS library_source,
+  null AS library_strategy
+UNION ALL
+with st
+MATCH (file)
+WHERE (file:sequencing_file OR file:pathology_file OR file:methylation_array_file OR file:single_cell_sequencing_file OR file:cytogenomic_file)
+MATCH (st)&lt;-[:of_cell_line|of_pdx]-(cl)&lt;--(sm:sample)
+Where (cl: cell_line or cl: pdx)
+MATCH (sm)&lt;--(file)
+OPTIONAL MATCH (st)&lt;-[:of_publication]-(pub:publication)
+OPTIONAL MATCH (st)&lt;--(p:participant)&lt;-[:of_diagnosis]-(dg:diagnosis)
+OPTIONAL MATCH (st)&lt;--(p)&lt;-[:of_follow_up]-(fu:follow_up)
+OPTIONAL MATCH (st)&lt;-[:of_study_personnel]-(stp:study_personnel)
+OPTIONAL MATCH (st)&lt;-[:of_study_funding]-(stf:study_funding)
+with file, sm, st, fu, dg, stf, stp
+RETURN DISTINCT
+  file.id as id,
+  null as pid,
+  CASE LABELS(file)[0]
+        WHEN 'sequencing_file' THEN file.sequencing_file_id
+        WHEN 'single_cell_sequencing_file' THEN file.single_cell_sequencing_file_id
+        WHEN 'cytogenomic_file' THEN file.cytogenomic_file_id
+        WHEN 'pathology_file' THEN file.pathology_file_id
+        WHEN 'methylation_array_file' THEN file.methylation_array_file_id END AS file_id,
+  file.dcf_indexd_guid AS guid,
+  file.file_name AS file_name,
+  CASE LABELS(file)[0]
+        WHEN 'sequencing_file' THEN 'Sequencing'
+        WHEN 'single_cell_sequencing_file' THEN 'Single Cell Sequencing'
+        WHEN 'cytogenomic_file' THEN 'Cytogenomic'
+        WHEN 'pathology_file' THEN 'Pathology imaging'
+        WHEN 'methylation_array_file' THEN 'Methylation array' END AS file_category,
+  file.file_type AS file_type,
+  file.file_description AS file_description,
+  file.file_size AS file_size,
+  file.md5sum AS md5sum,
+  st.study_id AS study_id,
+  st.phs_accession as phs_accession,
+  st.study_acronym as study_acronym,
+  st.study_short_title as study_short_title,
+  null AS participant_id,
+  sm.sample_id AS sample_id,
+  null as combined_filters,
+  null AS participant_filters,
+  COLLECT(DISTINCT {
+      age_at_diagnosis: dg.age_at_diagnosis,
+      diagnosis_anatomic_site: dg.anatomic_site,
+      disease_phase: dg.disease_phase,
+      diagnosis_classification_system: dg.diagnosis_classification_system,
+      diagnosis_verification_status: dg.diagnosis_verification_status,
+      diagnosis_basis: dg.diagnosis_basis,
+      diagnosis_comment: dg.diagnosis_comment,
+      diagnosis_classification: dg.diagnosis_classification
+  }) AS diagnosis_filters,
+  COLLECT(DISTINCT fu.vital_status) as vital_status,
+  COLLECT(DISTINCT {
+      sample_anatomic_site: sm.anatomic_site,
+      participant_age_at_collection: sm.participant_age_at_collection,
+      sample_tumor_status: sm.sample_tumor_status,
+      tumor_classification: sm.tumor_classification
+  }) AS sample_filters,
+  COLLECT(DISTINCT stf.grant_id) as grant_id,
+  COLLECT(DISTINCT stp.institution) as institution,
+  CASE LABELS(file)[0]
+            WHEN 'sequencing_file' THEN file.library_selection
+            WHEN 'single_cell_sequencing_file' THEN file.library_selection
+            ELSE null END AS library_selection,
+  CASE LABELS(file)[0]
+            WHEN 'sequencing_file' THEN file.library_source
+            WHEN 'single_cell_sequencing_file' THEN file.library_source
+            ELSE null END AS library_source,
+  CASE LABELS(file)[0]
+            WHEN 'sequencing_file' THEN file.library_strategy
+            WHEN 'single_cell_sequencing_file' THEN file.library_strategy
+            ELSE null END AS library_strategy
+}
+with id, guid, file_name, file_category, file_type, file_description, file_size, md5sum, study_id, phs_accession, study_acronym, study_short_title, participant_id, sample_id, participant_filters,diagnosis_filters, vital_status, sample_filters, grant_id, institution,library_selection,library_source,library_strategy
+unwind participant_filters as participant_filter
+with id, guid, file_name, file_category, file_type, file_description, file_size, md5sum, study_id, phs_accession, study_acronym, study_short_title, participant_id, sample_id, participant_filter,diagnosis_filters, vital_status, sample_filters, grant_id, institution,library_selection,library_source,library_strategy
+ unwind diagnosis_filters as diagnosis_filter
+with id, guid, file_name, file_category, file_type, file_description, file_size, md5sum, study_id, phs_accession, study_acronym, study_short_title, participant_id, sample_id,diagnosis_filter, vital_status, sample_filters, grant_id, institution,library_selection,library_source,library_strategy
+ with id, guid, file_name, file_category, file_type, file_description, file_size, md5sum, study_id, phs_accession, study_acronym, study_short_title, participant_id, sample_id, vital_status, sample_filters, grant_id, institution,library_selection,library_source,library_strategy
+ unwind sample_filters as sample_filter
+with id, guid, file_name, file_category, file_type, file_description, file_size, md5sum, study_id, phs_accession, study_acronym, study_short_title, participant_id, sample_id, sample_filter, grant_id, institution,library_selection,library_source,library_strategy
+ with distinct id, guid, file_name, file_category, file_type, file_description, file_size, md5sum, study_id, phs_accession, study_acronym, study_short_title, participant_id, sample_id, grant_id, institution,library_selection,library_source,library_strategy
+call {
+  with id, guid, file_name, file_category, file_type, file_description, file_size, md5sum, study_id, phs_accession, study_acronym, study_short_title, participant_id, sample_id, grant_id, institution,library_selection,library_source,library_strategy
+  return id as fid, guid as dig, file_name as fn, file_category as fc, file_type as ft, file_description as fd, file_size as fsize, md5sum as md5, study_id as sid, phs_accession as pa, study_acronym as sa, study_short_title as sst, participant_id as pid, sample_id as smid, grant_id as gid, institution as istt,library_selection as ls,library_source as lis,library_strategy as listr
+  UNION ALL
+  with study_id
+  MATCH (file:clinical_measure_file)
+  MATCH (stu:study)&lt;-[:of_clinical_measure_file]-(file)
+  where stu.study_id = study_id
+  OPTIONAL MATCH (stu)&lt;-[:of_study_personnel]-(stp:study_personnel)
+  OPTIONAL MATCH (stu)&lt;-[:of_study_funding]-(stf:study_funding)
+  With file, stu, stf, stp
+  RETURN DISTINCT
+    file.id as fid,
+    file.dcf_indexd_guid AS dig,
+    file.file_name AS fn,
+    'Clinical data' AS fc,
+    file.file_type AS ft,
+    file.file_description AS fd,
+    file.file_size AS fsize,
+    file.md5sum AS md5,
+    stu.study_id AS sid,
+    stu.phs_accession as pa,
+    stu.study_acronym as sa,
+    stu.study_short_title as sst,
+    null AS pid,
+    null AS smid,
+    COLLECT(DISTINCT stf.grant_id) as gid,
+    COLLECT(DISTINCT stp.institution) as istt,
+    null AS ls,
+    null AS lis,
+    null AS listr
+}
+with fid as id, dig as guid, fn as file_name, fc as file_category, ft as file_type, fd as file_description, fsize as file_size, md5 as md5sum, sid as study_id, pa as phs_accession, sa as study_acronym, sst as study_short_title, pid as participant_id, smid as sample_id, gid as grant_id, istt as institution,ls as library_selection,lis as library_source,listr as library_strategy
+where ANY(element IN ['University of Southern California'] WHERE element IN institution)    and library_selection in ['PolyA']  
+with id, guid, file_name, file_category, file_type, file_description, file_size, ['Bytes', 'KB', 'MB', 'GB', 'TB'] AS units,
+        toInteger(floor(log(file_size)/log(1024))) as i,
+        2 as precision, md5sum, study_id, phs_accession, study_acronym, study_short_title, participant_id, sample_id, grant_id, institution,library_selection,library_source,library_strategy
+with id, guid, file_name, file_category, file_type, file_description, file_size, file_size /(1024^i) AS value,
+        10^precision AS factor,
+        units[i] as unit, md5sum, study_id, phs_accession, study_acronym, study_short_title, participant_id, sample_id, grant_id, institution,library_selection,library_source,library_strategy
+with id, guid, file_name, file_category, file_type, file_description, unit,
+        round(factor * value)/factor AS size, md5sum, study_id, phs_accession, study_acronym, study_short_title, participant_id, sample_id, grant_id, institution,library_selection,library_source,library_strategy     
+with DISTINCT id,
+        file_name,
+        file_category,
+        file_description,
+        file_type,
+        CASE size % 1 WHEN 0 THEN apoc.convert.toInteger(size)+' ' +unit ELSE size+' ' +unit END AS file_size_new,
+        study_id,
+        participant_id,
+        sample_id,
+        guid,
+        md5sum
+RETURN file_name AS `File Name`,
+file_category As `File Category`,
+file_description As `File Description`,
+file_type As `File Type`,
+file_size_new As `File Size`,
+study_id As `Study ID`,
+coalesce(participant_id, '') As `Participant ID`,
+coalesce(sample_id, '') As `Sample ID`,
+guid As `GUID`,
+md5sum As `MD5Sum`
+ORDER BY file_name LIMIT 100</t>
   </si>
 </sst>
 </file>
@@ -2416,8 +2417,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2451,16 +2452,16 @@
         <v>5</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:5" s="1" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
@@ -2468,16 +2469,16 @@
         <v>6</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:5" s="1" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
@@ -2485,16 +2486,16 @@
         <v>7</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:5" s="1" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
@@ -2502,16 +2503,16 @@
         <v>8</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:5" s="1" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
@@ -2519,16 +2520,16 @@
         <v>9</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" s="2" t="s">
+      <c r="E6" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>